<commit_message>
Add results of FFNN day ahead with WD and time
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33637\Documents\11. Deep Learning\2. Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BE2FAB-A7C7-410D-AA89-20C2D012EDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B77E2E-1786-4E66-947C-E5607367D8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,44 @@
     <sheet name="Day Ahead" sheetId="1" r:id="rId1"/>
     <sheet name="Intra Day" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4E8999E3-B0E2-488B-9900-9360228FB54F}</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{4E8999E3-B0E2-488B-9900-9360228FB54F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    With u an v for wind direction. Same results again without ws, but only u and v.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Model</t>
   </si>
@@ -89,6 +116,9 @@
   </si>
   <si>
     <t>Past power 24h + Forecast 1h WS + WD + time</t>
+  </si>
+  <si>
+    <t>24 past power</t>
   </si>
 </sst>
 </file>
@@ -98,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +142,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -160,6 +196,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="33637053650" id="{F33EF54D-F342-4A73-A6B9-D9FE37A0C54A}" userId="993b84f116c69144" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,12 +465,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D3" dT="2021-11-14T14:36:14.74" personId="{F33EF54D-F342-4A73-A6B9-D9FE37A0C54A}" id="{4E8999E3-B0E2-488B-9900-9360228FB54F}">
+    <text>With u an v for wind direction. Same results again without ws, but only u and v.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -437,7 +487,7 @@
     <col min="3" max="3" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,31 +498,43 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2" s="3">
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.17899999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>0.16800000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -480,7 +542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -488,7 +550,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -496,8 +558,17 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -506,7 +577,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>